<commit_message>
UPDATE truc a alex + feuille de temps
</commit_message>
<xml_diff>
--- a/Équipe1.xlsx
+++ b/Équipe1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="85">
   <si>
     <t>Membres</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Réunion PROF</t>
   </si>
   <si>
-    <t>DCO + DS</t>
-  </si>
-  <si>
     <t>Manipulation de BD</t>
   </si>
   <si>
@@ -261,6 +258,27 @@
   </si>
   <si>
     <t>Continuer ajouter jeu</t>
+  </si>
+  <si>
+    <t>DCO + DS + DN</t>
+  </si>
+  <si>
+    <t>Progammation Employe</t>
+  </si>
+  <si>
+    <t>Documentation DCC Equipe</t>
+  </si>
+  <si>
+    <t>1ere Recontre pacakage test</t>
+  </si>
+  <si>
+    <t>1ème Recontre pacakage test</t>
+  </si>
+  <si>
+    <t>Continuer la base de données Employe</t>
+  </si>
+  <si>
+    <t>Prototype interface papier test</t>
   </si>
 </sst>
 </file>
@@ -1734,8 +1752,8 @@
   </sheetPr>
   <dimension ref="B3:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,27 +1820,27 @@
       </c>
       <c r="J5" s="15">
         <f>SUMIF($C5:$C60,J$4,$F$5:$F$60)</f>
-        <v>5.5</v>
+        <v>10.5</v>
       </c>
       <c r="K5" s="15">
         <f t="shared" ref="K5:N5" si="0">SUMIF($C5:$C60,K$4,$F$5:$F$60)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L5" s="15">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="M5" s="15">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N5" s="15">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="O5" s="15">
         <f>SUMIF($C5:$C60,O$4,$F$5:$F$60)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="18" x14ac:dyDescent="0.35">
@@ -1929,23 +1947,23 @@
       </c>
       <c r="J9" s="15">
         <f>SUMIF($D5:$D60,J$8,$F$5:$F$60)</f>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" ref="K9:P9" si="1">SUMIF($D5:$D60,K$8,$F$5:$F$60)</f>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N9" s="15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="O9" s="15">
         <f t="shared" si="1"/>
@@ -2222,10 +2240,10 @@
         <v>15</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F25" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -2239,7 +2257,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="16">
         <v>1.5</v>
@@ -2256,7 +2274,7 @@
         <v>15</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="16">
         <v>0.5</v>
@@ -2273,7 +2291,7 @@
         <v>18</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" s="16">
         <v>0.5</v>
@@ -2290,7 +2308,7 @@
         <v>18</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="16">
         <v>0.5</v>
@@ -2307,7 +2325,7 @@
         <v>23</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="16">
         <v>0.5</v>
@@ -2324,7 +2342,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" s="16">
         <v>0.5</v>
@@ -2341,7 +2359,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="16">
         <v>0.5</v>
@@ -2358,7 +2376,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" s="16">
         <v>1</v>
@@ -2375,7 +2393,7 @@
         <v>16</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="16">
         <v>1</v>
@@ -2392,7 +2410,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="16">
         <v>0.5</v>
@@ -2409,7 +2427,7 @@
         <v>16</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="16">
         <v>4</v>
@@ -2426,7 +2444,7 @@
         <v>16</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" s="16">
         <v>3</v>
@@ -2443,7 +2461,7 @@
         <v>15</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="16">
         <v>1.5</v>
@@ -2460,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F39" s="16">
         <v>1</v>
@@ -2477,74 +2495,164 @@
         <v>16</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="16"/>
+      <c r="B41" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="12"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="16"/>
+      <c r="B42" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="12"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="16"/>
+      <c r="B43" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="12"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="16"/>
+      <c r="B44" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="12"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="16"/>
+      <c r="B45" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="12"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="16"/>
+      <c r="B46" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="12"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="16"/>
+      <c r="B47" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="12"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="16"/>
+      <c r="B48" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="12"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="16"/>
+      <c r="B49" s="12">
+        <v>42284</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="12"/>

</xml_diff>

<commit_message>
UPDATE EQUIPE feuille de temps
</commit_message>
<xml_diff>
--- a/Équipe1.xlsx
+++ b/Équipe1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="129">
   <si>
     <t>Membres</t>
   </si>
@@ -326,6 +326,93 @@
   </si>
   <si>
     <t>Prog equipe</t>
+  </si>
+  <si>
+    <t>Script des vues et des fonctions</t>
+  </si>
+  <si>
+    <t>Prog jeu</t>
+  </si>
+  <si>
+    <t>Rerouler les scripts, arranger des triggers, CRE_Package_Test commencé et CTE_Package_Test aussi</t>
+  </si>
+  <si>
+    <t>Arranger script insertion complet jeu et rouler scripts</t>
+  </si>
+  <si>
+    <t>arranger script insertion personnel et continuer CRE&amp;CTE</t>
+  </si>
+  <si>
+    <t>gossage personnel</t>
+  </si>
+  <si>
+    <t>Arranger classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finition package 1 </t>
+  </si>
+  <si>
+    <t>interface cas de test et projet</t>
+  </si>
+  <si>
+    <t>SCRUM</t>
+  </si>
+  <si>
+    <t>Apprendre ASP</t>
+  </si>
+  <si>
+    <t>Arranger BD</t>
+  </si>
+  <si>
+    <t>Répondre aux questions des équipiers</t>
+  </si>
+  <si>
+    <t>Test interface apprentissage ASP</t>
+  </si>
+  <si>
+    <t>Programmer groupe d'utilisateur</t>
+  </si>
+  <si>
+    <t>DCC-DCR package3</t>
+  </si>
+  <si>
+    <t>Fin des test du package 1 pis un peu du package 2</t>
+  </si>
+  <si>
+    <t>Correction de DN</t>
+  </si>
+  <si>
+    <t>Pour le package 3</t>
+  </si>
+  <si>
+    <t>Package3</t>
+  </si>
+  <si>
+    <t>Diviser les requetes du package 1</t>
+  </si>
+  <si>
+    <t>Plus d'analyse sur le package 3(DN,DC, pis interface)</t>
+  </si>
+  <si>
+    <t>Rencontre pour package 3</t>
+  </si>
+  <si>
+    <t>Prog Authentification</t>
+  </si>
+  <si>
+    <t>Prog Utilisateur</t>
+  </si>
+  <si>
+    <t>Concorder BD et Prog (fixer après rencontre client)</t>
+  </si>
+  <si>
+    <t>Prog utilisateurs</t>
+  </si>
+  <si>
+    <t>Finition prog Utilisateurs</t>
+  </si>
+  <si>
+    <t>Finition prog authentification</t>
   </si>
 </sst>
 </file>
@@ -491,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -510,6 +597,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,7 +1898,7 @@
   </sheetPr>
   <dimension ref="B3:P62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2924,13 +3023,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="45.88671875" customWidth="1"/>
+    <col min="5" max="5" width="47.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2995,7 +3094,7 @@
       </c>
       <c r="L5" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M5" s="15">
         <f t="shared" si="0"/>
@@ -3003,7 +3102,7 @@
       </c>
       <c r="N5" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O5" s="15">
         <f>SUMIF($C5:$C60,O$4,$F$5:$F$60)</f>
@@ -3118,11 +3217,11 @@
       </c>
       <c r="K9" s="15">
         <f t="shared" ref="K9:P9" si="1">SUMIF($D5:$D60,K$8,$F$5:$F$60)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="1"/>
@@ -3244,95 +3343,225 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="12">
+        <v>42287</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="12">
+        <v>42287</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="16"/>
+      <c r="B18" s="12">
+        <v>42288</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="16"/>
+      <c r="B19" s="12">
+        <v>42291</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18">
+        <v>42291</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="16"/>
+      <c r="B21" s="12">
+        <v>42292</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="12">
+        <v>42292</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="16"/>
+      <c r="B23" s="12">
+        <v>42293</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="16"/>
+      <c r="B24" s="12">
+        <v>42293</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="16"/>
+      <c r="B25" s="12">
+        <v>42290</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="16"/>
+      <c r="B26" s="12">
+        <v>42294</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
+      <c r="B27" s="12">
+        <v>42294</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="12"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="16"/>
+      <c r="B28" s="12">
+        <v>42290</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
@@ -3576,10 +3805,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P60"/>
+  <dimension ref="B3:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3640,28 +3869,28 @@
         <v>5</v>
       </c>
       <c r="J5" s="15">
-        <f>SUMIF($C5:$C60,J$4,$F$5:$F$60)</f>
-        <v>0</v>
+        <f>SUMIF($C5:$C59,J$4,$F$5:$F$59)</f>
+        <v>4</v>
       </c>
       <c r="K5" s="15">
-        <f t="shared" ref="K5:N5" si="0">SUMIF($C5:$C60,K$4,$F$5:$F$60)</f>
-        <v>11</v>
+        <f>SUMIF($C5:$C59,K$4,$F$5:$F$59)</f>
+        <v>26.5</v>
       </c>
       <c r="L5" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUMIF($C5:$C59,L$4,$F$5:$F$59)</f>
+        <v>20</v>
       </c>
       <c r="M5" s="15">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUMIF($C5:$C59,M$4,$F$5:$F$59)</f>
+        <v>17.5</v>
       </c>
       <c r="N5" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUMIF($C5:$C59,N$4,$F$5:$F$59)</f>
+        <v>12</v>
       </c>
       <c r="O5" s="15">
-        <f>SUMIF($C5:$C60,O$4,$F$5:$F$60)</f>
-        <v>0</v>
+        <f>SUMIF($C5:$C59,O$4,$F$5:$F$59)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="18" x14ac:dyDescent="0.35">
@@ -3767,31 +3996,31 @@
         <v>1</v>
       </c>
       <c r="J9" s="15">
-        <f>SUMIF($D5:$D60,J$8,$F$5:$F$60)</f>
+        <f>SUMIF($D5:$D59,J$8,$F$5:$F$59)</f>
+        <v>6.5</v>
+      </c>
+      <c r="K9" s="15">
+        <f>SUMIF($D5:$D59,K$8,$F$5:$F$59)</f>
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="15">
+        <f>SUMIF($D5:$D59,L$8,$F$5:$F$59)</f>
+        <v>60</v>
+      </c>
+      <c r="M9" s="15">
+        <f>SUMIF($D5:$D59,M$8,$F$5:$F$59)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="15">
-        <f t="shared" ref="K9:P9" si="1">SUMIF($D5:$D60,K$8,$F$5:$F$60)</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="15">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="M9" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N9" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUMIF($D5:$D59,N$8,$F$5:$F$59)</f>
+        <v>3.5</v>
       </c>
       <c r="O9" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUMIF($D5:$D59,O$8,$F$5:$F$59)</f>
+        <v>23.5</v>
       </c>
       <c r="P9" s="15">
-        <f t="shared" si="1"/>
+        <f>SUMIF($D5:$D59,P$8,$F$5:$F$59)</f>
         <v>0</v>
       </c>
     </row>
@@ -3813,305 +4042,735 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="16"/>
+      <c r="B11" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="16">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="16"/>
+      <c r="B12" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="16"/>
+      <c r="B13" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="16"/>
+      <c r="B14" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="16"/>
+      <c r="B15" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="16"/>
+      <c r="B18" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="16"/>
+      <c r="B19" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="16"/>
+      <c r="B20" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="16"/>
+      <c r="B21" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="16"/>
+      <c r="B23" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="16"/>
+      <c r="B24" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="16"/>
+      <c r="B25" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="16"/>
+      <c r="B26" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
+      <c r="B27" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="12"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="16"/>
+      <c r="B28" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="12"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="16"/>
+      <c r="B29" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="12"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="16"/>
+      <c r="B30" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="12"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="16"/>
+      <c r="B31" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="12"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="16"/>
+      <c r="B32" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="12"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="16"/>
+      <c r="B33" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="16"/>
+      <c r="B34" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="12"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="16"/>
+      <c r="B35" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="12"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="16"/>
+      <c r="B36" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="16"/>
+      <c r="B37" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="12"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="16"/>
+      <c r="B38" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="12"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="16"/>
+      <c r="B39" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="12"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="16"/>
+      <c r="B40" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="16"/>
+      <c r="B41" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="16">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="12"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="16"/>
+      <c r="B42" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="12"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="16"/>
+      <c r="B43" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="12"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="16"/>
+      <c r="B44" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="12"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="16"/>
+      <c r="B45" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="16">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="12"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="16"/>
+      <c r="B46" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="16">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="12"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="16"/>
+      <c r="B47" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="12"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="16"/>
+      <c r="B48" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="12"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="16"/>
+      <c r="B49" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="12"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="16"/>
+      <c r="B50" s="12">
+        <v>42296</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="12"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="16"/>
+      <c r="B51" s="12">
+        <v>42297</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="16">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="12"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="16"/>
+      <c r="B52" s="12">
+        <v>42298</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F52" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="12"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="16"/>
+      <c r="B53" s="12">
+        <v>42299</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F53" s="16">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="12"/>
@@ -4155,22 +4814,15 @@
       <c r="E59" s="1"/>
       <c r="F59" s="16"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="12"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="16"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Temps" prompt="Entrez le temps accordée à cette tâche" sqref="F5:F60">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Temps" prompt="Entrez le temps accordée à cette tâche" sqref="F5:F59">
       <formula1>Temps</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Code Catégories" error="Saisir code dans la liste" promptTitle="Code de Catégories" prompt="Saisir code de la catégorie" sqref="D5:D60">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Code Catégories" error="Saisir code dans la liste" promptTitle="Code de Catégories" prompt="Saisir code de la catégorie" sqref="D5:D59">
       <formula1>Code</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Membre non valide" promptTitle="Membres" prompt="Saisir votre nom" sqref="C5:C60">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Membre non valide" promptTitle="Membres" prompt="Saisir votre nom" sqref="C5:C59">
       <formula1>Membres</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>